<commit_message>
Sankey app with scenarios
</commit_message>
<xml_diff>
--- a/results/flows_per_year.xlsx
+++ b/results/flows_per_year.xlsx
@@ -441,82 +441,82 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>F_0_1_t</t>
+          <t>F_0_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>F_1_2_t</t>
+          <t>F_1_2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>F_1_9_t</t>
+          <t>F_1_9</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>F_2_3_t</t>
+          <t>F_2_3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>F_3_4_t</t>
+          <t>F_3_4</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F_4_0_t</t>
+          <t>F_4_0</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>F_4_5_t</t>
+          <t>F_4_5</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>F_4_7_t</t>
+          <t>F_4_7</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>F_5_6_t</t>
+          <t>F_5_6</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>F_5_7_t</t>
+          <t>F_5_7</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>F_6_0_t</t>
+          <t>F_6_0</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>F_6_1_t</t>
+          <t>F_6_1</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>F_7_0_t</t>
+          <t>F_7_0</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>F_7_1_t</t>
+          <t>F_7_1</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>F_7_8_t</t>
+          <t>F_7_8</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>F_8_1_t</t>
+          <t>F_8_1</t>
         </is>
       </c>
     </row>

</xml_diff>